<commit_message>
change deadlines to future date
</commit_message>
<xml_diff>
--- a/organisation/organisation-test.xlsx
+++ b/organisation/organisation-test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklastodenhoefer/py_projects_git/Organisation/task_organisation_and_plotting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklastodenhoefer/py_projects_git/Organisation/project_task_analysis/organisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D394CAD-8E90-6649-BD9A-142109FB74DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F06F467-900B-AC45-BB6F-A56869955EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="35340" windowHeight="17900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="30580" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -73,12 +73,51 @@
     <t>Effort (hrs)</t>
   </si>
   <si>
+    <t>Unnamed: 17</t>
+  </si>
+  <si>
+    <t>Big Data Fundamentals with PySpark 100%</t>
+  </si>
+  <si>
+    <t>School budgeting with Machine Learning</t>
+  </si>
+  <si>
+    <t>CiSo: Prep Affordable Housing lecture</t>
+  </si>
+  <si>
+    <t>Big Data Fundamentals with PySpark 50%</t>
+  </si>
+  <si>
+    <t>Intro to Seaborn</t>
+  </si>
+  <si>
+    <t>Intro to Visualization</t>
+  </si>
+  <si>
+    <t>Machine Learning with PySpark</t>
+  </si>
+  <si>
+    <t>plot overdone tasks as bubble scatterplot separately</t>
+  </si>
+  <si>
+    <t>Finish MT Car Sharing Blockchain</t>
+  </si>
+  <si>
+    <t>Read 4 Paper</t>
+  </si>
+  <si>
+    <t>calculate daily recurring tasks</t>
+  </si>
+  <si>
     <t>140 chars YT to Bear</t>
   </si>
   <si>
     <t>Prep L1 CiSo</t>
   </si>
   <si>
+    <t xml:space="preserve">MT register topic&amp;partner </t>
+  </si>
+  <si>
     <t>Dash small dashboard with two graphics</t>
   </si>
   <si>
@@ -88,67 +127,28 @@
     <t>Day Countdown</t>
   </si>
   <si>
+    <t>.epub + LDA (one chapter content)</t>
+  </si>
+  <si>
+    <t>Online course</t>
+  </si>
+  <si>
+    <t>Uni</t>
+  </si>
+  <si>
     <t>Coding</t>
   </si>
   <si>
-    <t>Uni</t>
+    <t>Medium</t>
   </si>
   <si>
     <t>Done</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>To-Do</t>
   </si>
   <si>
     <t>Doing</t>
-  </si>
-  <si>
-    <t>Big Data Fundamentals with PySpark 100%</t>
-  </si>
-  <si>
-    <t>Online course</t>
-  </si>
-  <si>
-    <t>Irrelevant</t>
-  </si>
-  <si>
-    <t>CiSo: Prep Affordable Housing lecture</t>
-  </si>
-  <si>
-    <t>Big Data Fundamentals with PySpark 50%</t>
-  </si>
-  <si>
-    <t>Intro to Seaborn</t>
-  </si>
-  <si>
-    <t>Intro to Visualization</t>
-  </si>
-  <si>
-    <t>plot overdone tasks as bubble scatterplot separately</t>
-  </si>
-  <si>
-    <t>Finish MT Car Sharing Blockchain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT register topic&amp;partner </t>
-  </si>
-  <si>
-    <t>.epub + LDA (one chapter content)</t>
-  </si>
-  <si>
-    <t>Read 4 Paper</t>
-  </si>
-  <si>
-    <t>School budgeting with Machine Learning</t>
-  </si>
-  <si>
-    <t>Machine Learning with PySpark</t>
-  </si>
-  <si>
-    <t>calculate daily recurring tasks</t>
   </si>
 </sst>
 </file>
@@ -158,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,14 +170,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,20 +207,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -565,16 +554,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="7" width="15.6640625" customWidth="1"/>
@@ -585,7 +574,7 @@
     <col min="17" max="17" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,22 +626,25 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2">
         <v>44353.904861111107</v>
       </c>
       <c r="E2" s="2">
-        <v>44537.916666666664</v>
+        <v>44537.916666666657</v>
       </c>
       <c r="F2">
         <v>18</v>
@@ -670,31 +662,30 @@
         <v>4</v>
       </c>
       <c r="K2">
-        <v>-100</v>
+        <v>78</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="2"/>
+        <v>39</v>
+      </c>
       <c r="P2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D3" s="2">
         <v>44081.869444444441</v>
       </c>
       <c r="E3" s="2">
-        <v>44089.833333333343</v>
+        <v>44819.833333333336</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -715,36 +706,33 @@
         <v>-100</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+        <v>40</v>
+      </c>
       <c r="O3">
         <v>192.68</v>
       </c>
       <c r="P3" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="Q3">
         <v>29.55</v>
       </c>
-      <c r="R3" s="3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2">
         <v>44081.759722222218</v>
       </c>
       <c r="E4" s="2">
-        <v>44083.958333333343</v>
+        <v>44813.958333333336</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -765,35 +753,33 @@
         <v>-100</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+        <v>40</v>
+      </c>
       <c r="O4">
         <v>49.73</v>
       </c>
       <c r="P4" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="Q4">
         <v>2.25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2">
         <v>44100.74722222222</v>
       </c>
       <c r="E5" s="2">
-        <v>44362.916666666657</v>
+        <v>44727.916666666664</v>
       </c>
       <c r="F5">
         <v>67</v>
@@ -814,34 +800,33 @@
         <v>-100</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5" s="2"/>
+        <v>40</v>
+      </c>
       <c r="O5">
         <v>6075.78</v>
       </c>
       <c r="P5" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="Q5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2">
         <v>44079.79791666667</v>
       </c>
       <c r="E6" s="2">
-        <v>44082.75</v>
+        <v>44812.75</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -862,35 +847,33 @@
         <v>-100</v>
       </c>
       <c r="L6" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+        <v>40</v>
+      </c>
       <c r="O6">
         <v>49.72</v>
       </c>
       <c r="P6" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="Q6">
         <v>31.87</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2">
         <v>44078.660416666673</v>
       </c>
       <c r="E7" s="2">
-        <v>44080.583333333343</v>
+        <v>44810.583333333336</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -911,34 +894,33 @@
         <v>-100</v>
       </c>
       <c r="L7" t="s">
-        <v>30</v>
-      </c>
-      <c r="N7" s="2"/>
+        <v>40</v>
+      </c>
       <c r="O7">
         <v>27.25</v>
       </c>
       <c r="P7" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="Q7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D8" s="2">
         <v>44129.064583333333</v>
       </c>
       <c r="E8" s="2">
-        <v>44364.833333333343</v>
+        <v>44729.833333333336</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -959,35 +941,33 @@
         <v>-100</v>
       </c>
       <c r="L8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N8" s="2"/>
+        <v>40</v>
+      </c>
       <c r="O8">
         <v>5444.95</v>
       </c>
       <c r="P8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="Q8">
         <v>4</v>
       </c>
-      <c r="S8" s="3"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2">
         <v>44132.660416666673</v>
       </c>
       <c r="E9" s="2">
-        <v>44614.916666666664</v>
+        <v>44614.916666666657</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1005,33 +985,33 @@
         <v>3</v>
       </c>
       <c r="K9">
-        <v>-100</v>
+        <v>75</v>
       </c>
       <c r="L9" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="P9" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="Q9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2">
         <v>44077.992361111108</v>
       </c>
       <c r="E10" s="2">
-        <v>44091.583333333343</v>
+        <v>44821.583333333336</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1052,34 +1032,33 @@
         <v>-100</v>
       </c>
       <c r="L10" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" s="2"/>
+        <v>40</v>
+      </c>
       <c r="O10">
         <v>326.97000000000003</v>
       </c>
       <c r="P10" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="Q10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D11" s="2">
         <v>44077.989583333343</v>
       </c>
       <c r="E11" s="2">
-        <v>44091.666666666657</v>
+        <v>44821.666666666664</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1100,35 +1079,33 @@
         <v>-100</v>
       </c>
       <c r="L11" t="s">
-        <v>30</v>
-      </c>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+        <v>40</v>
+      </c>
       <c r="O11">
         <v>330.63</v>
       </c>
       <c r="P11" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="Q11">
         <v>2.85</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2">
         <v>44073.577962962961</v>
       </c>
       <c r="E12" s="2">
-        <v>44374.833333333343</v>
+        <v>44739.833333333336</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1149,30 +1126,30 @@
         <v>95</v>
       </c>
       <c r="L12" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="P12" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="Q12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2">
         <v>44073.569560185177</v>
       </c>
       <c r="E13" s="2">
-        <v>44088.708333333343</v>
+        <v>44088.708333333336</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1193,7 +1170,7 @@
         <v>-100</v>
       </c>
       <c r="L13" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="M13" s="2">
         <v>44074.625</v>
@@ -1205,21 +1182,21 @@
         <v>313.52999999999997</v>
       </c>
       <c r="P13" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="Q13">
         <v>288.2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D14" s="2">
         <v>44073.560532407413</v>
@@ -1246,7 +1223,7 @@
         <v>-100</v>
       </c>
       <c r="L14" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="N14" s="2">
         <v>44077.812893518523</v>
@@ -1255,21 +1232,18 @@
         <v>102.06</v>
       </c>
       <c r="P14" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
       <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
       </c>
       <c r="D15" s="2">
         <v>44073.432604166657</v>
@@ -1296,7 +1270,7 @@
         <v>-100</v>
       </c>
       <c r="L15" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="M15" s="2">
         <v>44148.375</v>
@@ -1308,21 +1282,21 @@
         <v>1800.62</v>
       </c>
       <c r="P15" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="Q15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2">
         <v>44073.431377314817</v>
@@ -1349,7 +1323,7 @@
         <v>-100</v>
       </c>
       <c r="L16" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="M16" s="2">
         <v>44141.965277777781</v>
@@ -1361,7 +1335,7 @@
         <v>1645.75</v>
       </c>
       <c r="P16" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="Q16">
         <v>0.93</v>
@@ -1372,10 +1346,10 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D17" s="2">
         <v>44073.106168981481</v>
@@ -1402,7 +1376,7 @@
         <v>-100</v>
       </c>
       <c r="L17" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="M17" s="2">
         <v>44087.666666666657</v>
@@ -1414,7 +1388,7 @@
         <v>351.12</v>
       </c>
       <c r="P17" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="Q17">
         <v>1.67</v>
@@ -1425,10 +1399,10 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D18" s="2">
         <v>44073.105624999997</v>
@@ -1455,7 +1429,7 @@
         <v>-100</v>
       </c>
       <c r="L18" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="N18" s="2">
         <v>44075.583333333343</v>
@@ -1464,10 +1438,7 @@
         <v>59.47</v>
       </c>
       <c r="P18" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q18">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
@@ -1475,10 +1446,10 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
         <v>38</v>
-      </c>
-      <c r="C19" t="s">
-        <v>22</v>
       </c>
       <c r="D19" s="2">
         <v>44072.462280092594</v>
@@ -1505,13 +1476,13 @@
         <v>98</v>
       </c>
       <c r="L19" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="M19" s="2">
         <v>44075.583333333343</v>
       </c>
       <c r="P19" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>